<commit_message>
changes on result made and email sending done
</commit_message>
<xml_diff>
--- a/excel DB format/Courses.xlsx
+++ b/excel DB format/Courses.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="296">
   <si>
     <t>code</t>
   </si>
@@ -4588,12 +4588,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F272"/>
+  <dimension ref="A1:F284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B100" sqref="B100"/>
+      <selection pane="bottomLeft" activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -8829,10 +8829,10 @@
     </row>
     <row r="212" ht="18" spans="1:6">
       <c r="A212" s="5" t="s">
-        <v>195</v>
+        <v>68</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>196</v>
+        <v>69</v>
       </c>
       <c r="C212" s="6">
         <v>2</v>
@@ -8844,15 +8844,15 @@
         <v>7</v>
       </c>
       <c r="F212" s="1">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="213" ht="18" spans="1:6">
       <c r="A213" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C213" s="6">
         <v>2</v>
@@ -8869,13 +8869,13 @@
     </row>
     <row r="214" ht="18" spans="1:6">
       <c r="A214" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C214" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D214" s="1" t="s">
         <v>8</v>
@@ -8889,10 +8889,10 @@
     </row>
     <row r="215" ht="18" spans="1:6">
       <c r="A215" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C215" s="6">
         <v>3</v>
@@ -8909,10 +8909,10 @@
     </row>
     <row r="216" ht="18" spans="1:6">
       <c r="A216" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C216" s="6">
         <v>3</v>
@@ -8929,10 +8929,10 @@
     </row>
     <row r="217" ht="18" spans="1:6">
       <c r="A217" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C217" s="6">
         <v>3</v>
@@ -8949,10 +8949,10 @@
     </row>
     <row r="218" ht="18" spans="1:6">
       <c r="A218" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C218" s="6">
         <v>3</v>
@@ -8968,14 +8968,14 @@
       </c>
     </row>
     <row r="219" ht="18" spans="1:6">
-      <c r="A219" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B219" s="8" t="s">
-        <v>136</v>
+      <c r="A219" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B219" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="C219" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>8</v>
@@ -8988,11 +8988,11 @@
       </c>
     </row>
     <row r="220" ht="18" spans="1:6">
-      <c r="A220" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B220" s="5" t="s">
-        <v>67</v>
+      <c r="A220" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="C220" s="6">
         <v>2</v>
@@ -9001,18 +9001,18 @@
         <v>8</v>
       </c>
       <c r="E220" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F220" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="221" ht="18" spans="1:6">
       <c r="A221" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>209</v>
+        <v>67</v>
       </c>
       <c r="C221" s="6">
         <v>2</v>
@@ -9029,10 +9029,10 @@
     </row>
     <row r="222" ht="18" spans="1:6">
       <c r="A222" s="5" t="s">
-        <v>210</v>
+        <v>146</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C222" s="6">
         <v>2</v>
@@ -9049,10 +9049,10 @@
     </row>
     <row r="223" ht="18" spans="1:6">
       <c r="A223" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C223" s="6">
         <v>2</v>
@@ -9069,10 +9069,10 @@
     </row>
     <row r="224" ht="18" spans="1:6">
       <c r="A224" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C224" s="6">
         <v>2</v>
@@ -9089,10 +9089,10 @@
     </row>
     <row r="225" ht="18" spans="1:6">
       <c r="A225" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C225" s="6">
         <v>2</v>
@@ -9109,10 +9109,10 @@
     </row>
     <row r="226" ht="18" spans="1:6">
       <c r="A226" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C226" s="6">
         <v>2</v>
@@ -9129,10 +9129,10 @@
     </row>
     <row r="227" ht="18" spans="1:6">
       <c r="A227" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C227" s="6">
         <v>2</v>
@@ -9149,10 +9149,10 @@
     </row>
     <row r="228" ht="18" spans="1:6">
       <c r="A228" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C228" s="6">
         <v>2</v>
@@ -9169,10 +9169,10 @@
     </row>
     <row r="229" ht="18" spans="1:6">
       <c r="A229" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C229" s="6">
         <v>2</v>
@@ -9181,7 +9181,7 @@
         <v>8</v>
       </c>
       <c r="E229" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F229" s="1">
         <v>200</v>
@@ -9189,10 +9189,10 @@
     </row>
     <row r="230" ht="18" spans="1:6">
       <c r="A230" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C230" s="6">
         <v>2</v>
@@ -9209,10 +9209,10 @@
     </row>
     <row r="231" ht="18" spans="1:6">
       <c r="A231" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C231" s="6">
         <v>2</v>
@@ -9229,10 +9229,10 @@
     </row>
     <row r="232" ht="18" spans="1:6">
       <c r="A232" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C232" s="6">
         <v>2</v>
@@ -9249,10 +9249,10 @@
     </row>
     <row r="233" ht="18" spans="1:6">
       <c r="A233" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C233" s="6">
         <v>2</v>
@@ -9269,10 +9269,10 @@
     </row>
     <row r="234" ht="18" spans="1:6">
       <c r="A234" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C234" s="6">
         <v>2</v>
@@ -9289,10 +9289,10 @@
     </row>
     <row r="235" ht="18" spans="1:6">
       <c r="A235" s="5" t="s">
-        <v>62</v>
+        <v>234</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>177</v>
+        <v>235</v>
       </c>
       <c r="C235" s="6">
         <v>2</v>
@@ -9309,10 +9309,10 @@
     </row>
     <row r="236" ht="18" spans="1:6">
       <c r="A236" s="5" t="s">
-        <v>145</v>
+        <v>62</v>
       </c>
       <c r="B236" s="5" t="s">
-        <v>67</v>
+        <v>177</v>
       </c>
       <c r="C236" s="6">
         <v>2</v>
@@ -9329,10 +9329,10 @@
     </row>
     <row r="237" ht="18" spans="1:6">
       <c r="A237" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C237" s="6">
         <v>2</v>
@@ -9349,33 +9349,33 @@
     </row>
     <row r="238" ht="18" spans="1:6">
       <c r="A238" s="5" t="s">
-        <v>236</v>
+        <v>146</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>237</v>
+        <v>69</v>
       </c>
       <c r="C238" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E238" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F238" s="1">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="239" ht="18" spans="1:6">
       <c r="A239" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C239" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D239" s="1" t="s">
         <v>8</v>
@@ -9389,10 +9389,10 @@
     </row>
     <row r="240" ht="18" spans="1:6">
       <c r="A240" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C240" s="6">
         <v>2</v>
@@ -9409,10 +9409,10 @@
     </row>
     <row r="241" ht="18" spans="1:6">
       <c r="A241" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C241" s="6">
         <v>2</v>
@@ -9429,13 +9429,13 @@
     </row>
     <row r="242" ht="18" spans="1:6">
       <c r="A242" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="B242" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="C242" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D242" s="1" t="s">
         <v>8</v>
@@ -9449,13 +9449,13 @@
     </row>
     <row r="243" ht="18" spans="1:6">
       <c r="A243" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B243" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
+      </c>
+      <c r="B243" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="C243" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D243" s="1" t="s">
         <v>8</v>
@@ -9469,10 +9469,10 @@
     </row>
     <row r="244" ht="18" spans="1:6">
       <c r="A244" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C244" s="6">
         <v>2</v>
@@ -9489,10 +9489,10 @@
     </row>
     <row r="245" ht="18" spans="1:6">
       <c r="A245" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C245" s="6">
         <v>2</v>
@@ -9509,13 +9509,13 @@
     </row>
     <row r="246" ht="18" spans="1:6">
       <c r="A246" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C246" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D246" s="1" t="s">
         <v>8</v>
@@ -9529,13 +9529,13 @@
     </row>
     <row r="247" ht="18" spans="1:6">
       <c r="A247" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C247" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D247" s="1" t="s">
         <v>8</v>
@@ -9548,14 +9548,14 @@
       </c>
     </row>
     <row r="248" ht="18" spans="1:6">
-      <c r="A248" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B248" s="8" t="s">
-        <v>136</v>
+      <c r="A248" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="C248" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D248" s="1" t="s">
         <v>8</v>
@@ -9568,20 +9568,20 @@
       </c>
     </row>
     <row r="249" ht="18" spans="1:6">
-      <c r="A249" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B249" s="5" t="s">
-        <v>237</v>
+      <c r="A249" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B249" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="C249" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D249" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E249" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F249" s="1">
         <v>300</v>
@@ -9589,10 +9589,10 @@
     </row>
     <row r="250" ht="18" spans="1:6">
       <c r="A250" s="5" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="C250" s="6">
         <v>3</v>
@@ -9609,13 +9609,13 @@
     </row>
     <row r="251" ht="18" spans="1:6">
       <c r="A251" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C251" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D251" s="1" t="s">
         <v>8</v>
@@ -9629,13 +9629,13 @@
     </row>
     <row r="252" ht="18" spans="1:6">
       <c r="A252" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="B252" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="C252" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D252" s="1" t="s">
         <v>8</v>
@@ -9649,10 +9649,10 @@
     </row>
     <row r="253" ht="18" spans="1:6">
       <c r="A253" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="B253" s="12" t="s">
-        <v>245</v>
+        <v>260</v>
+      </c>
+      <c r="B253" s="11" t="s">
+        <v>261</v>
       </c>
       <c r="C253" s="6">
         <v>3</v>
@@ -9669,10 +9669,10 @@
     </row>
     <row r="254" ht="18" spans="1:6">
       <c r="A254" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="B254" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
+      </c>
+      <c r="B254" s="12" t="s">
+        <v>245</v>
       </c>
       <c r="C254" s="6">
         <v>3</v>
@@ -9689,13 +9689,13 @@
     </row>
     <row r="255" ht="18" spans="1:6">
       <c r="A255" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C255" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D255" s="1" t="s">
         <v>8</v>
@@ -9709,13 +9709,13 @@
     </row>
     <row r="256" ht="18" spans="1:6">
       <c r="A256" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C256" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>8</v>
@@ -9729,10 +9729,10 @@
     </row>
     <row r="257" ht="18" spans="1:6">
       <c r="A257" s="5" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>237</v>
+        <v>268</v>
       </c>
       <c r="C257" s="6">
         <v>3</v>
@@ -9741,7 +9741,7 @@
         <v>8</v>
       </c>
       <c r="E257" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F257" s="1">
         <v>300</v>
@@ -9749,13 +9749,13 @@
     </row>
     <row r="258" ht="18" spans="1:6">
       <c r="A258" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="B258" s="7" t="s">
-        <v>245</v>
+        <v>236</v>
+      </c>
+      <c r="B258" s="5" t="s">
+        <v>237</v>
       </c>
       <c r="C258" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D258" s="1" t="s">
         <v>8</v>
@@ -9769,10 +9769,10 @@
     </row>
     <row r="259" ht="18" spans="1:6">
       <c r="A259" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="B259" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
+      </c>
+      <c r="B259" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="C259" s="6">
         <v>2</v>
@@ -9789,13 +9789,13 @@
     </row>
     <row r="260" ht="18" spans="1:6">
       <c r="A260" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C260" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D260" s="1" t="s">
         <v>8</v>
@@ -9809,13 +9809,13 @@
     </row>
     <row r="261" ht="18" spans="1:6">
       <c r="A261" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="B261" s="11" t="s">
-        <v>275</v>
+        <v>272</v>
+      </c>
+      <c r="B261" s="5" t="s">
+        <v>273</v>
       </c>
       <c r="C261" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D261" s="1" t="s">
         <v>8</v>
@@ -9829,10 +9829,10 @@
     </row>
     <row r="262" ht="18" spans="1:6">
       <c r="A262" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B262" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C262" s="6">
         <v>2</v>
@@ -9849,13 +9849,13 @@
     </row>
     <row r="263" ht="18" spans="1:6">
       <c r="A263" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="B263" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
+      </c>
+      <c r="B263" s="11" t="s">
+        <v>277</v>
       </c>
       <c r="C263" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D263" s="1" t="s">
         <v>8</v>
@@ -9869,13 +9869,13 @@
     </row>
     <row r="264" ht="18" spans="1:6">
       <c r="A264" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C264" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D264" s="1" t="s">
         <v>8</v>
@@ -9889,13 +9889,13 @@
     </row>
     <row r="265" ht="18" spans="1:6">
       <c r="A265" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C265" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D265" s="1" t="s">
         <v>8</v>
@@ -9908,11 +9908,11 @@
       </c>
     </row>
     <row r="266" ht="18" spans="1:6">
-      <c r="A266" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B266" s="8" t="s">
-        <v>136</v>
+      <c r="A266" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B266" s="5" t="s">
+        <v>283</v>
       </c>
       <c r="C266" s="6">
         <v>2</v>
@@ -9928,31 +9928,31 @@
       </c>
     </row>
     <row r="267" ht="18" spans="1:6">
-      <c r="A267" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B267" s="5" t="s">
-        <v>285</v>
+      <c r="A267" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B267" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="C267" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D267" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E267" s="1">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F267" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="268" ht="18" spans="1:6">
       <c r="A268" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C268" s="6">
         <v>3</v>
@@ -9969,10 +9969,10 @@
     </row>
     <row r="269" ht="18" spans="1:6">
       <c r="A269" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C269" s="6">
         <v>3</v>
@@ -9989,13 +9989,13 @@
     </row>
     <row r="270" ht="18" spans="1:6">
       <c r="A270" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C270" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D270" s="1" t="s">
         <v>8</v>
@@ -10009,13 +10009,13 @@
     </row>
     <row r="271" ht="18" spans="1:6">
       <c r="A271" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C271" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D271" s="1" t="s">
         <v>8</v>
@@ -10029,10 +10029,10 @@
     </row>
     <row r="272" ht="18" spans="1:6">
       <c r="A272" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C272" s="6">
         <v>3</v>
@@ -10045,6 +10045,246 @@
       </c>
       <c r="F272" s="1">
         <v>400</v>
+      </c>
+    </row>
+    <row r="273" ht="18" spans="1:6">
+      <c r="A273" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B273" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C273" s="6">
+        <v>3</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E273" s="1">
+        <v>17</v>
+      </c>
+      <c r="F273" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="274" ht="18" spans="1:6">
+      <c r="A274" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B274" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C274" s="6">
+        <v>3</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E274" s="1">
+        <v>16</v>
+      </c>
+      <c r="F274" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="275" ht="18" spans="1:6">
+      <c r="A275" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B275" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C275" s="6">
+        <v>1</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E275" s="1">
+        <v>16</v>
+      </c>
+      <c r="F275" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="276" ht="18" spans="1:6">
+      <c r="A276" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B276" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C276" s="6">
+        <v>3</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E276" s="1">
+        <v>16</v>
+      </c>
+      <c r="F276" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="277" ht="18" spans="1:6">
+      <c r="A277" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B277" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C277" s="6">
+        <v>3</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E277" s="1">
+        <v>16</v>
+      </c>
+      <c r="F277" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="278" ht="18" spans="1:6">
+      <c r="A278" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B278" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C278" s="6">
+        <v>3</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E278" s="1">
+        <v>16</v>
+      </c>
+      <c r="F278" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="279" ht="18" spans="1:6">
+      <c r="A279" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B279" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C279" s="6">
+        <v>1</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E279" s="1">
+        <v>16</v>
+      </c>
+      <c r="F279" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="280" ht="18" spans="1:6">
+      <c r="A280" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B280" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C280" s="6">
+        <v>2</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E280" s="1">
+        <v>16</v>
+      </c>
+      <c r="F280" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="281" ht="18" spans="1:6">
+      <c r="A281" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B281" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C281" s="6">
+        <v>2</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E281" s="1">
+        <v>16</v>
+      </c>
+      <c r="F281" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="282" ht="18" spans="1:6">
+      <c r="A282" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C282" s="6">
+        <v>2</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E282" s="1">
+        <v>16</v>
+      </c>
+      <c r="F282" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="283" ht="18" spans="1:6">
+      <c r="A283" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B283" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C283" s="6">
+        <v>2</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E283" s="1">
+        <v>16</v>
+      </c>
+      <c r="F283" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="284" ht="18" spans="1:6">
+      <c r="A284" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B284" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C284" s="6">
+        <v>2</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E284" s="1">
+        <v>16</v>
+      </c>
+      <c r="F284" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>